<commit_message>
updated files 09:02pm 11/02/2025
</commit_message>
<xml_diff>
--- a/Tabelas com os resultados dos testes -12-01-2025/Level1TestcaseReport.xlsx
+++ b/Tabelas com os resultados dos testes -12-01-2025/Level1TestcaseReport.xlsx
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,6 +383,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,11 +699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332968248"/>
-        <c:axId val="332969424"/>
+        <c:axId val="338412856"/>
+        <c:axId val="338408936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332968248"/>
+        <c:axId val="338412856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332969424"/>
+        <c:crossAx val="338408936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332969424"/>
+        <c:axId val="338408936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332968248"/>
+        <c:crossAx val="338412856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1278,11 +1281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334550928"/>
-        <c:axId val="334552496"/>
+        <c:axId val="340759480"/>
+        <c:axId val="340759872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334550928"/>
+        <c:axId val="340759480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334552496"/>
+        <c:crossAx val="340759872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1333,7 +1336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334552496"/>
+        <c:axId val="340759872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1384,7 +1387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334550928"/>
+        <c:crossAx val="340759480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1398,6 +1401,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1821,11 +1825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334553672"/>
-        <c:axId val="332965112"/>
+        <c:axId val="340765752"/>
+        <c:axId val="338415600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334553672"/>
+        <c:axId val="340765752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332965112"/>
+        <c:crossAx val="338415600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1876,7 +1880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332965112"/>
+        <c:axId val="338415600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1927,7 +1931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334553672"/>
+        <c:crossAx val="340765752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1941,6 +1945,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2292,11 +2297,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332966288"/>
-        <c:axId val="332966680"/>
+        <c:axId val="338410112"/>
+        <c:axId val="338410504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332966288"/>
+        <c:axId val="338410112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2339,7 +2344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332966680"/>
+        <c:crossAx val="338410504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2347,7 +2352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332966680"/>
+        <c:axId val="338410504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +2403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332966288"/>
+        <c:crossAx val="338410112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2412,6 +2417,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2835,11 +2841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335485024"/>
-        <c:axId val="335486200"/>
+        <c:axId val="341216464"/>
+        <c:axId val="341210976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335485024"/>
+        <c:axId val="341216464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2882,7 +2888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335486200"/>
+        <c:crossAx val="341210976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2890,7 +2896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335486200"/>
+        <c:axId val="341210976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,7 +2947,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335485024"/>
+        <c:crossAx val="341216464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2955,6 +2961,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3378,11 +3385,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335479536"/>
-        <c:axId val="335483064"/>
+        <c:axId val="341210584"/>
+        <c:axId val="341215288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335479536"/>
+        <c:axId val="341210584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3425,7 +3432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335483064"/>
+        <c:crossAx val="341215288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3433,7 +3440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335483064"/>
+        <c:axId val="341215288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3484,7 +3491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335479536"/>
+        <c:crossAx val="341210584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3498,6 +3505,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3874,11 +3882,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="335478752"/>
-        <c:axId val="335483848"/>
+        <c:axId val="341214112"/>
+        <c:axId val="341209016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335478752"/>
+        <c:axId val="341214112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3921,7 +3929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335483848"/>
+        <c:crossAx val="341209016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3929,7 +3937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335483848"/>
+        <c:axId val="341209016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3980,7 +3988,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335478752"/>
+        <c:crossAx val="341214112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4346,11 +4354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335484240"/>
-        <c:axId val="335484632"/>
+        <c:axId val="341211368"/>
+        <c:axId val="341211760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335484240"/>
+        <c:axId val="341211368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4393,7 +4401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335484632"/>
+        <c:crossAx val="341211760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4401,7 +4409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335484632"/>
+        <c:axId val="341211760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4452,7 +4460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335484240"/>
+        <c:crossAx val="341211368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4818,11 +4826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335481104"/>
-        <c:axId val="335482280"/>
+        <c:axId val="341209408"/>
+        <c:axId val="341212544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335481104"/>
+        <c:axId val="341209408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4865,7 +4873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335482280"/>
+        <c:crossAx val="341212544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4873,7 +4881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335482280"/>
+        <c:axId val="341212544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4924,7 +4932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335481104"/>
+        <c:crossAx val="341209408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5290,11 +5298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335481888"/>
-        <c:axId val="335482672"/>
+        <c:axId val="341212936"/>
+        <c:axId val="341213328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335481888"/>
+        <c:axId val="341212936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5337,7 +5345,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335482672"/>
+        <c:crossAx val="341213328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5345,7 +5353,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335482672"/>
+        <c:axId val="341213328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5396,7 +5404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335481888"/>
+        <c:crossAx val="341212936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5762,11 +5770,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335480320"/>
-        <c:axId val="362690360"/>
+        <c:axId val="341213720"/>
+        <c:axId val="364172520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335480320"/>
+        <c:axId val="341213720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5809,7 +5817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362690360"/>
+        <c:crossAx val="364172520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5817,7 +5825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362690360"/>
+        <c:axId val="364172520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +5876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335480320"/>
+        <c:crossAx val="341213720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6234,11 +6242,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332962760"/>
-        <c:axId val="332968640"/>
+        <c:axId val="338413248"/>
+        <c:axId val="338414032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332962760"/>
+        <c:axId val="338413248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6281,7 +6289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332968640"/>
+        <c:crossAx val="338414032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6289,7 +6297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332968640"/>
+        <c:axId val="338414032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6340,7 +6348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332962760"/>
+        <c:crossAx val="338413248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6730,11 +6738,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="362688792"/>
-        <c:axId val="362692712"/>
+        <c:axId val="364174480"/>
+        <c:axId val="364172128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362688792"/>
+        <c:axId val="364174480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6777,7 +6785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362692712"/>
+        <c:crossAx val="364172128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6785,7 +6793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362692712"/>
+        <c:axId val="364172128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6836,7 +6844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362688792"/>
+        <c:crossAx val="364174480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7274,11 +7282,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362693104"/>
-        <c:axId val="362686832"/>
+        <c:axId val="364175656"/>
+        <c:axId val="364176440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362693104"/>
+        <c:axId val="364175656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7321,7 +7329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362686832"/>
+        <c:crossAx val="364176440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7329,7 +7337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362686832"/>
+        <c:axId val="364176440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7380,7 +7388,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362693104"/>
+        <c:crossAx val="364175656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7818,11 +7826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362689184"/>
-        <c:axId val="362687616"/>
+        <c:axId val="364176832"/>
+        <c:axId val="364172912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362689184"/>
+        <c:axId val="364176832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7865,7 +7873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362687616"/>
+        <c:crossAx val="364172912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7873,7 +7881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362687616"/>
+        <c:axId val="364172912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7924,7 +7932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362689184"/>
+        <c:crossAx val="364176832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8362,11 +8370,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362688008"/>
-        <c:axId val="362691536"/>
+        <c:axId val="364176048"/>
+        <c:axId val="364170952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362688008"/>
+        <c:axId val="364176048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8409,7 +8417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362691536"/>
+        <c:crossAx val="364170952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8417,7 +8425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362691536"/>
+        <c:axId val="364170952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8468,7 +8476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362688008"/>
+        <c:crossAx val="364176048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8906,11 +8914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362693496"/>
-        <c:axId val="362692320"/>
+        <c:axId val="364170560"/>
+        <c:axId val="364171344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362693496"/>
+        <c:axId val="364170560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8953,7 +8961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362692320"/>
+        <c:crossAx val="364171344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8961,7 +8969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362692320"/>
+        <c:axId val="364171344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9012,7 +9020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362693496"/>
+        <c:crossAx val="364170560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9450,11 +9458,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362693888"/>
-        <c:axId val="362689968"/>
+        <c:axId val="364169776"/>
+        <c:axId val="364174872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362693888"/>
+        <c:axId val="364169776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9497,7 +9505,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362689968"/>
+        <c:crossAx val="364174872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9505,7 +9513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362689968"/>
+        <c:axId val="364174872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9556,7 +9564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362693888"/>
+        <c:crossAx val="364169776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9994,11 +10002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362930696"/>
-        <c:axId val="362924424"/>
+        <c:axId val="364649392"/>
+        <c:axId val="364644296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362930696"/>
+        <c:axId val="364649392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10041,7 +10049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362924424"/>
+        <c:crossAx val="364644296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10049,7 +10057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362924424"/>
+        <c:axId val="364644296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10100,7 +10108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362930696"/>
+        <c:crossAx val="364649392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10466,11 +10474,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362929520"/>
-        <c:axId val="362927952"/>
+        <c:axId val="364649784"/>
+        <c:axId val="364650176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362929520"/>
+        <c:axId val="364649784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10513,7 +10521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362927952"/>
+        <c:crossAx val="364650176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10521,7 +10529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362927952"/>
+        <c:axId val="364650176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10572,7 +10580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362929520"/>
+        <c:crossAx val="364649784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10586,7 +10594,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10938,11 +10945,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362927168"/>
-        <c:axId val="362931480"/>
+        <c:axId val="364649000"/>
+        <c:axId val="364644688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362927168"/>
+        <c:axId val="364649000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10985,7 +10992,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362931480"/>
+        <c:crossAx val="364644688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10993,7 +11000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362931480"/>
+        <c:axId val="364644688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11044,7 +11051,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362927168"/>
+        <c:crossAx val="364649000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11058,7 +11065,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11410,11 +11416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362930304"/>
-        <c:axId val="362929912"/>
+        <c:axId val="364643512"/>
+        <c:axId val="364645080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362930304"/>
+        <c:axId val="364643512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11457,7 +11463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362929912"/>
+        <c:crossAx val="364645080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11465,7 +11471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362929912"/>
+        <c:axId val="364645080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11516,7 +11522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362930304"/>
+        <c:crossAx val="364643512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11530,7 +11536,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11882,11 +11887,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332965504"/>
-        <c:axId val="332961976"/>
+        <c:axId val="338411288"/>
+        <c:axId val="338415992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332965504"/>
+        <c:axId val="338411288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11929,7 +11934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332961976"/>
+        <c:crossAx val="338415992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11937,7 +11942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332961976"/>
+        <c:axId val="338415992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11988,7 +11993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332965504"/>
+        <c:crossAx val="338411288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12353,11 +12358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362931872"/>
-        <c:axId val="362927560"/>
+        <c:axId val="364643904"/>
+        <c:axId val="364645864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362931872"/>
+        <c:axId val="364643904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12400,7 +12405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362927560"/>
+        <c:crossAx val="364645864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12408,7 +12413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362927560"/>
+        <c:axId val="364645864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12459,7 +12464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362931872"/>
+        <c:crossAx val="364643904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12473,7 +12478,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12897,11 +12901,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362924816"/>
-        <c:axId val="362925600"/>
+        <c:axId val="364646648"/>
+        <c:axId val="364647040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362924816"/>
+        <c:axId val="364646648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12944,7 +12948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362925600"/>
+        <c:crossAx val="364647040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12952,7 +12956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362925600"/>
+        <c:axId val="364647040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13003,7 +13007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362924816"/>
+        <c:crossAx val="364646648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13017,7 +13021,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13441,11 +13444,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362928344"/>
-        <c:axId val="362928736"/>
+        <c:axId val="364648216"/>
+        <c:axId val="364648608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362928344"/>
+        <c:axId val="364648216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13488,7 +13491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362928736"/>
+        <c:crossAx val="364648608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13496,7 +13499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362928736"/>
+        <c:axId val="364648608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13547,7 +13550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362928344"/>
+        <c:crossAx val="364648216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13561,7 +13564,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14010,11 +14012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="362790232"/>
-        <c:axId val="362789448"/>
+        <c:axId val="365178040"/>
+        <c:axId val="365179608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362790232"/>
+        <c:axId val="365178040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14057,7 +14059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362789448"/>
+        <c:crossAx val="365179608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14065,7 +14067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362789448"/>
+        <c:axId val="365179608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14116,7 +14118,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362790232"/>
+        <c:crossAx val="365178040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14130,7 +14132,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14554,11 +14555,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362788664"/>
-        <c:axId val="362791408"/>
+        <c:axId val="365176472"/>
+        <c:axId val="365180000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362788664"/>
+        <c:axId val="365176472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14601,7 +14602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362791408"/>
+        <c:crossAx val="365180000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14609,7 +14610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362791408"/>
+        <c:axId val="365180000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14660,7 +14661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362788664"/>
+        <c:crossAx val="365176472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14674,7 +14675,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15098,11 +15098,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="362789840"/>
-        <c:axId val="362791800"/>
+        <c:axId val="365180392"/>
+        <c:axId val="365179216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="362789840"/>
+        <c:axId val="365180392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15145,7 +15145,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362791800"/>
+        <c:crossAx val="365179216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15153,7 +15153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362791800"/>
+        <c:axId val="365179216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15204,7 +15204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362789840"/>
+        <c:crossAx val="365180392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15218,7 +15218,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15642,11 +15641,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="363648488"/>
-        <c:axId val="363650056"/>
+        <c:axId val="365181568"/>
+        <c:axId val="365180784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="363648488"/>
+        <c:axId val="365181568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15689,7 +15688,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363650056"/>
+        <c:crossAx val="365180784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15697,7 +15696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="363650056"/>
+        <c:axId val="365180784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15748,7 +15747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363648488"/>
+        <c:crossAx val="365181568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15762,7 +15761,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16114,11 +16112,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332963152"/>
-        <c:axId val="332963544"/>
+        <c:axId val="338412072"/>
+        <c:axId val="338414816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332963152"/>
+        <c:axId val="338412072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16161,7 +16159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332963544"/>
+        <c:crossAx val="338414816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16169,7 +16167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332963544"/>
+        <c:axId val="338414816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16220,7 +16218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332963152"/>
+        <c:crossAx val="338412072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16657,11 +16655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334553280"/>
-        <c:axId val="334555632"/>
+        <c:axId val="340762616"/>
+        <c:axId val="340763008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334553280"/>
+        <c:axId val="340762616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16704,7 +16702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334555632"/>
+        <c:crossAx val="340763008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16712,7 +16710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334555632"/>
+        <c:axId val="340763008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16763,7 +16761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334553280"/>
+        <c:crossAx val="340762616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17200,11 +17198,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334556808"/>
-        <c:axId val="334555240"/>
+        <c:axId val="340763792"/>
+        <c:axId val="340761832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334556808"/>
+        <c:axId val="340763792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17247,7 +17245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334555240"/>
+        <c:crossAx val="340761832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17255,7 +17253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334555240"/>
+        <c:axId val="340761832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17306,7 +17304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334556808"/>
+        <c:crossAx val="340763792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17681,11 +17679,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334554456"/>
-        <c:axId val="334554064"/>
+        <c:axId val="340761048"/>
+        <c:axId val="340766144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334554456"/>
+        <c:axId val="340761048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17728,7 +17726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334554064"/>
+        <c:crossAx val="340766144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17736,7 +17734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334554064"/>
+        <c:axId val="340766144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17787,7 +17785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334554456"/>
+        <c:crossAx val="340761048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17840,6 +17838,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18191,11 +18190,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334556416"/>
-        <c:axId val="334557200"/>
+        <c:axId val="340764576"/>
+        <c:axId val="340766928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334556416"/>
+        <c:axId val="340764576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18238,7 +18237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334557200"/>
+        <c:crossAx val="340766928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18246,7 +18245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334557200"/>
+        <c:axId val="340766928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18297,7 +18296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334556416"/>
+        <c:crossAx val="340764576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18311,6 +18310,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18734,11 +18734,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334550144"/>
-        <c:axId val="334551320"/>
+        <c:axId val="340761440"/>
+        <c:axId val="340764184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334550144"/>
+        <c:axId val="340761440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18781,7 +18781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334551320"/>
+        <c:crossAx val="340764184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18789,7 +18789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334551320"/>
+        <c:axId val="340764184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18840,7 +18840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334550144"/>
+        <c:crossAx val="340761440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18854,6 +18854,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -48864,8 +48865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:F227"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F8"/>
+    <sheetView topLeftCell="A147" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -51763,7 +51764,8 @@
     <mergeCell ref="B123:F124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -51771,8 +51773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:F329"/>
   <sheetViews>
-    <sheetView topLeftCell="A294" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="R325" sqref="R325"/>
+    <sheetView topLeftCell="A10" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -56076,16 +56078,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B252:C252"/>
+    <mergeCell ref="B279:C280"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B201:C202"/>
+    <mergeCell ref="B150:F151"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B42:F43"/>
     <mergeCell ref="B69:F70"/>
     <mergeCell ref="B96:F97"/>
     <mergeCell ref="B123:F124"/>
-    <mergeCell ref="B252:C252"/>
-    <mergeCell ref="B279:C280"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B201:C202"/>
-    <mergeCell ref="B150:F151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -56097,8 +56099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A15:F390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="I353" sqref="I353"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H382" sqref="H382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -60913,17 +60915,17 @@
     </row>
     <row r="369" spans="1:6">
       <c r="A369" s="20"/>
-      <c r="B369" s="23">
+      <c r="B369" s="34">
         <v>4.8872947692870997E-2</v>
       </c>
-      <c r="C369" s="23">
+      <c r="C369" s="34">
         <v>1</v>
       </c>
       <c r="D369" s="22"/>
-      <c r="E369" s="23">
+      <c r="E369" s="7">
         <v>2.1942138671875E-2</v>
       </c>
-      <c r="F369" s="23">
+      <c r="F369" s="7">
         <v>1</v>
       </c>
     </row>
@@ -61233,17 +61235,17 @@
     </row>
     <row r="389" spans="1:6">
       <c r="A389" s="20"/>
-      <c r="B389" s="23">
+      <c r="B389" s="8">
         <v>2.3329050540924001</v>
       </c>
-      <c r="C389" s="23">
+      <c r="C389" s="8">
         <v>100</v>
       </c>
       <c r="D389" s="22"/>
-      <c r="E389" s="23">
+      <c r="E389" s="8">
         <v>2.2951962947845401</v>
       </c>
-      <c r="F389" s="23">
+      <c r="F389" s="8">
         <v>100</v>
       </c>
     </row>
@@ -61257,17 +61259,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B15:F16"/>
+    <mergeCell ref="B42:F43"/>
+    <mergeCell ref="B69:F70"/>
+    <mergeCell ref="B95:F96"/>
+    <mergeCell ref="B122:C123"/>
     <mergeCell ref="B365:C366"/>
     <mergeCell ref="B283:C283"/>
     <mergeCell ref="B310:C311"/>
     <mergeCell ref="B174:C174"/>
     <mergeCell ref="B201:C202"/>
     <mergeCell ref="B256:C257"/>
-    <mergeCell ref="B15:F16"/>
-    <mergeCell ref="B42:F43"/>
-    <mergeCell ref="B69:F70"/>
-    <mergeCell ref="B95:F96"/>
-    <mergeCell ref="B122:C123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated files 11:04pm 12/02/2025
</commit_message>
<xml_diff>
--- a/Tabelas com os resultados dos testes -12-01-2025/Level1TestcaseReport.xlsx
+++ b/Tabelas com os resultados dos testes -12-01-2025/Level1TestcaseReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="7275" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1 Guest (1-100MB)" sheetId="13" r:id="rId1"/>
@@ -362,6 +362,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -382,9 +385,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,11 +699,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="338412856"/>
-        <c:axId val="338408936"/>
+        <c:axId val="334973224"/>
+        <c:axId val="334973608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338412856"/>
+        <c:axId val="334973224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338408936"/>
+        <c:crossAx val="334973608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338408936"/>
+        <c:axId val="334973608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,7 +805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338412856"/>
+        <c:crossAx val="334973224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -858,6 +858,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1281,11 +1282,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340759480"/>
-        <c:axId val="340759872"/>
+        <c:axId val="333573472"/>
+        <c:axId val="333566024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340759480"/>
+        <c:axId val="333573472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1329,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340759872"/>
+        <c:crossAx val="333566024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1337,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340759872"/>
+        <c:axId val="333566024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1388,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340759480"/>
+        <c:crossAx val="333573472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1825,11 +1826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340765752"/>
-        <c:axId val="338415600"/>
+        <c:axId val="335477504"/>
+        <c:axId val="335477896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340765752"/>
+        <c:axId val="335477504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,7 +1873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338415600"/>
+        <c:crossAx val="335477896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1880,7 +1881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338415600"/>
+        <c:axId val="335477896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1931,7 +1932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340765752"/>
+        <c:crossAx val="335477504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2297,11 +2298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="338410112"/>
-        <c:axId val="338410504"/>
+        <c:axId val="335478288"/>
+        <c:axId val="335480248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338410112"/>
+        <c:axId val="335478288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2345,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338410504"/>
+        <c:crossAx val="335480248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2352,7 +2353,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338410504"/>
+        <c:axId val="335480248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2403,7 +2404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338410112"/>
+        <c:crossAx val="335478288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2841,11 +2842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341216464"/>
-        <c:axId val="341210976"/>
+        <c:axId val="335479464"/>
+        <c:axId val="335481032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341216464"/>
+        <c:axId val="335479464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,7 +2889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341210976"/>
+        <c:crossAx val="335481032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2896,7 +2897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341210976"/>
+        <c:axId val="335481032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2947,7 +2948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341216464"/>
+        <c:crossAx val="335479464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3385,11 +3386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341210584"/>
-        <c:axId val="341215288"/>
+        <c:axId val="335481816"/>
+        <c:axId val="335482208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341210584"/>
+        <c:axId val="335481816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,7 +3433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341215288"/>
+        <c:crossAx val="335482208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3440,7 +3441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341215288"/>
+        <c:axId val="335482208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,7 +3492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341210584"/>
+        <c:crossAx val="335481816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3882,11 +3883,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="341214112"/>
-        <c:axId val="341209016"/>
+        <c:axId val="335478680"/>
+        <c:axId val="335479072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341214112"/>
+        <c:axId val="335478680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3929,7 +3930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341209016"/>
+        <c:crossAx val="335479072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3937,7 +3938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341209016"/>
+        <c:axId val="335479072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3988,7 +3989,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341214112"/>
+        <c:crossAx val="335478680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4002,7 +4003,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4354,11 +4354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341211368"/>
-        <c:axId val="341211760"/>
+        <c:axId val="335475544"/>
+        <c:axId val="335475936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341211368"/>
+        <c:axId val="335475544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4401,7 +4401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341211760"/>
+        <c:crossAx val="335475936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4409,7 +4409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341211760"/>
+        <c:axId val="335475936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4460,7 +4460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341211368"/>
+        <c:crossAx val="335475544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4474,7 +4474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4826,11 +4825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341209408"/>
-        <c:axId val="341212544"/>
+        <c:axId val="335477112"/>
+        <c:axId val="334201768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341209408"/>
+        <c:axId val="335477112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4873,7 +4872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341212544"/>
+        <c:crossAx val="334201768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4881,7 +4880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341212544"/>
+        <c:axId val="334201768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4932,7 +4931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341209408"/>
+        <c:crossAx val="335477112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4946,7 +4945,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5298,11 +5296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341212936"/>
-        <c:axId val="341213328"/>
+        <c:axId val="334200984"/>
+        <c:axId val="334195104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341212936"/>
+        <c:axId val="334200984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5345,7 +5343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341213328"/>
+        <c:crossAx val="334195104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5353,7 +5351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341213328"/>
+        <c:axId val="334195104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5404,7 +5402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341212936"/>
+        <c:crossAx val="334200984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5418,7 +5416,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5770,11 +5767,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341213720"/>
-        <c:axId val="364172520"/>
+        <c:axId val="334197848"/>
+        <c:axId val="334195888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341213720"/>
+        <c:axId val="334197848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5817,7 +5814,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364172520"/>
+        <c:crossAx val="334195888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5825,7 +5822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364172520"/>
+        <c:axId val="334195888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5876,7 +5873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341213720"/>
+        <c:crossAx val="334197848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5890,7 +5887,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6242,11 +6238,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="338413248"/>
-        <c:axId val="338414032"/>
+        <c:axId val="334444952"/>
+        <c:axId val="333845368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338413248"/>
+        <c:axId val="334444952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6289,7 +6285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338414032"/>
+        <c:crossAx val="333845368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6297,7 +6293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338414032"/>
+        <c:axId val="333845368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6348,7 +6344,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338413248"/>
+        <c:crossAx val="334444952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6362,6 +6358,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6738,11 +6735,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="364174480"/>
-        <c:axId val="364172128"/>
+        <c:axId val="334194320"/>
+        <c:axId val="334198240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364174480"/>
+        <c:axId val="334194320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6785,7 +6782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364172128"/>
+        <c:crossAx val="334198240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6793,7 +6790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364172128"/>
+        <c:axId val="334198240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6844,7 +6841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364174480"/>
+        <c:crossAx val="334194320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6858,7 +6855,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7282,11 +7278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364175656"/>
-        <c:axId val="364176440"/>
+        <c:axId val="334194712"/>
+        <c:axId val="334195496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364175656"/>
+        <c:axId val="334194712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7329,7 +7325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364176440"/>
+        <c:crossAx val="334195496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7337,7 +7333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364176440"/>
+        <c:axId val="334195496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7388,7 +7384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364175656"/>
+        <c:crossAx val="334194712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7402,7 +7398,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7826,11 +7821,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364176832"/>
-        <c:axId val="364172912"/>
+        <c:axId val="334198632"/>
+        <c:axId val="334196672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364176832"/>
+        <c:axId val="334198632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7873,7 +7868,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364172912"/>
+        <c:crossAx val="334196672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7881,7 +7876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364172912"/>
+        <c:axId val="334196672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7932,7 +7927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364176832"/>
+        <c:crossAx val="334198632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7946,7 +7941,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8370,11 +8364,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364176048"/>
-        <c:axId val="364170952"/>
+        <c:axId val="334199024"/>
+        <c:axId val="334199808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364176048"/>
+        <c:axId val="334199024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8417,7 +8411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364170952"/>
+        <c:crossAx val="334199808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8425,7 +8419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364170952"/>
+        <c:axId val="334199808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8476,7 +8470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364176048"/>
+        <c:crossAx val="334199024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8490,7 +8484,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8914,11 +8907,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364170560"/>
-        <c:axId val="364171344"/>
+        <c:axId val="362752168"/>
+        <c:axId val="362754128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364170560"/>
+        <c:axId val="362752168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8961,7 +8954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364171344"/>
+        <c:crossAx val="362754128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8969,7 +8962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364171344"/>
+        <c:axId val="362754128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9020,7 +9013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364170560"/>
+        <c:crossAx val="362752168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9034,7 +9027,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9458,11 +9450,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364169776"/>
-        <c:axId val="364174872"/>
+        <c:axId val="362756872"/>
+        <c:axId val="362755304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364169776"/>
+        <c:axId val="362756872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9505,7 +9497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364174872"/>
+        <c:crossAx val="362755304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9513,7 +9505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364174872"/>
+        <c:axId val="362755304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9564,7 +9556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364169776"/>
+        <c:crossAx val="362756872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9578,7 +9570,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10002,11 +9993,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364649392"/>
-        <c:axId val="364644296"/>
+        <c:axId val="362750992"/>
+        <c:axId val="362756088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364649392"/>
+        <c:axId val="362750992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10049,7 +10040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364644296"/>
+        <c:crossAx val="362756088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10057,7 +10048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364644296"/>
+        <c:axId val="362756088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10108,7 +10099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364649392"/>
+        <c:crossAx val="362750992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10122,7 +10113,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10474,11 +10464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364649784"/>
-        <c:axId val="364650176"/>
+        <c:axId val="362753344"/>
+        <c:axId val="362757264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364649784"/>
+        <c:axId val="362753344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10521,7 +10511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364650176"/>
+        <c:crossAx val="362757264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10529,7 +10519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364650176"/>
+        <c:axId val="362757264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10580,7 +10570,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364649784"/>
+        <c:crossAx val="362753344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10945,11 +10935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364649000"/>
-        <c:axId val="364644688"/>
+        <c:axId val="362754912"/>
+        <c:axId val="362755696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364649000"/>
+        <c:axId val="362754912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10992,7 +10982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364644688"/>
+        <c:crossAx val="362755696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11000,7 +10990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364644688"/>
+        <c:axId val="362755696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11051,7 +11041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364649000"/>
+        <c:crossAx val="362754912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11416,11 +11406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364643512"/>
-        <c:axId val="364645080"/>
+        <c:axId val="362751776"/>
+        <c:axId val="362753736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364643512"/>
+        <c:axId val="362751776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11463,7 +11453,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364645080"/>
+        <c:crossAx val="362753736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11471,7 +11461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364645080"/>
+        <c:axId val="362753736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11522,7 +11512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364643512"/>
+        <c:crossAx val="362751776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11887,11 +11877,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="338411288"/>
-        <c:axId val="338415992"/>
+        <c:axId val="334487512"/>
+        <c:axId val="334487896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338411288"/>
+        <c:axId val="334487512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11934,7 +11924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338415992"/>
+        <c:crossAx val="334487896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11942,7 +11932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338415992"/>
+        <c:axId val="334487896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11993,7 +11983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338411288"/>
+        <c:crossAx val="334487512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12007,6 +11997,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12358,11 +12349,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364643904"/>
-        <c:axId val="364645864"/>
+        <c:axId val="362751384"/>
+        <c:axId val="362752560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364643904"/>
+        <c:axId val="362751384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12405,7 +12396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364645864"/>
+        <c:crossAx val="362752560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12413,7 +12404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364645864"/>
+        <c:axId val="362752560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12464,7 +12455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364643904"/>
+        <c:crossAx val="362751384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12901,11 +12892,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364646648"/>
-        <c:axId val="364647040"/>
+        <c:axId val="335729888"/>
+        <c:axId val="335735768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364646648"/>
+        <c:axId val="335729888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12948,7 +12939,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364647040"/>
+        <c:crossAx val="335735768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12956,7 +12947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364647040"/>
+        <c:axId val="335735768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13007,7 +12998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364646648"/>
+        <c:crossAx val="335729888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13444,11 +13435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="364648216"/>
-        <c:axId val="364648608"/>
+        <c:axId val="335733024"/>
+        <c:axId val="335736160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="364648216"/>
+        <c:axId val="335733024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13491,7 +13482,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364648608"/>
+        <c:crossAx val="335736160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13499,7 +13490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364648608"/>
+        <c:axId val="335736160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13550,7 +13541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364648216"/>
+        <c:crossAx val="335733024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14012,11 +14003,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="365178040"/>
-        <c:axId val="365179608"/>
+        <c:axId val="335731456"/>
+        <c:axId val="335732240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365178040"/>
+        <c:axId val="335731456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14059,7 +14050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365179608"/>
+        <c:crossAx val="335732240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14067,7 +14058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365179608"/>
+        <c:axId val="335732240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14118,7 +14109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365178040"/>
+        <c:crossAx val="335731456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14555,11 +14546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="365176472"/>
-        <c:axId val="365180000"/>
+        <c:axId val="335733416"/>
+        <c:axId val="335733808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365176472"/>
+        <c:axId val="335733416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14602,7 +14593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365180000"/>
+        <c:crossAx val="335733808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14610,7 +14601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365180000"/>
+        <c:axId val="335733808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14661,7 +14652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365176472"/>
+        <c:crossAx val="335733416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15098,11 +15089,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="365180392"/>
-        <c:axId val="365179216"/>
+        <c:axId val="335734200"/>
+        <c:axId val="335730672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365180392"/>
+        <c:axId val="335734200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15145,7 +15136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365179216"/>
+        <c:crossAx val="335730672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15153,7 +15144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365179216"/>
+        <c:axId val="335730672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15204,7 +15195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365180392"/>
+        <c:crossAx val="335734200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15641,11 +15632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="365181568"/>
-        <c:axId val="365180784"/>
+        <c:axId val="335732632"/>
+        <c:axId val="335734592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="365181568"/>
+        <c:axId val="335732632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15688,7 +15679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365180784"/>
+        <c:crossAx val="335734592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15696,7 +15687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="365180784"/>
+        <c:axId val="335734592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15747,7 +15738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365181568"/>
+        <c:crossAx val="335732632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15761,6 +15752,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16112,11 +16104,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="338412072"/>
-        <c:axId val="338414816"/>
+        <c:axId val="334494936"/>
+        <c:axId val="334614192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="338412072"/>
+        <c:axId val="334494936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16159,7 +16151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338414816"/>
+        <c:crossAx val="334614192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16167,7 +16159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="338414816"/>
+        <c:axId val="334614192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16218,7 +16210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="338412072"/>
+        <c:crossAx val="334494936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16232,6 +16224,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16655,11 +16648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340762616"/>
-        <c:axId val="340763008"/>
+        <c:axId val="333567592"/>
+        <c:axId val="333568768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340762616"/>
+        <c:axId val="333567592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16702,7 +16695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340763008"/>
+        <c:crossAx val="333568768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16710,7 +16703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340763008"/>
+        <c:axId val="333568768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16761,7 +16754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340762616"/>
+        <c:crossAx val="333567592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16775,6 +16768,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17198,11 +17192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340763792"/>
-        <c:axId val="340761832"/>
+        <c:axId val="333569160"/>
+        <c:axId val="333566416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340763792"/>
+        <c:axId val="333569160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17245,7 +17239,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340761832"/>
+        <c:crossAx val="333566416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17253,7 +17247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340761832"/>
+        <c:axId val="333566416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17304,7 +17298,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340763792"/>
+        <c:crossAx val="333569160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17318,6 +17312,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17679,11 +17674,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340761048"/>
-        <c:axId val="340766144"/>
+        <c:axId val="333567984"/>
+        <c:axId val="333568376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340761048"/>
+        <c:axId val="333567984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17726,7 +17721,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340766144"/>
+        <c:crossAx val="333568376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17734,7 +17729,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340766144"/>
+        <c:axId val="333568376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17785,7 +17780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340761048"/>
+        <c:crossAx val="333567984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18190,11 +18185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340764576"/>
-        <c:axId val="340766928"/>
+        <c:axId val="333573080"/>
+        <c:axId val="333570728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340764576"/>
+        <c:axId val="333573080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18237,7 +18232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340766928"/>
+        <c:crossAx val="333570728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18245,7 +18240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340766928"/>
+        <c:axId val="333570728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18296,7 +18291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340764576"/>
+        <c:crossAx val="333573080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18734,11 +18729,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340761440"/>
-        <c:axId val="340764184"/>
+        <c:axId val="333571904"/>
+        <c:axId val="333572296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340761440"/>
+        <c:axId val="333571904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18781,7 +18776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340764184"/>
+        <c:crossAx val="333572296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18789,7 +18784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340764184"/>
+        <c:axId val="333572296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18840,7 +18835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340761440"/>
+        <c:crossAx val="333571904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -46325,7 +46320,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -46650,8 +46645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:F177"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView topLeftCell="A149" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156:F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -46674,30 +46669,30 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="3" t="s">
@@ -47046,27 +47041,27 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="29"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:6">
@@ -47402,20 +47397,20 @@
       </c>
     </row>
     <row r="71" spans="2:6">
-      <c r="B71" s="31" t="s">
+      <c r="B71" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
     </row>
     <row r="72" spans="2:6">
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
     </row>
     <row r="74" spans="2:6">
       <c r="B74" s="3" t="s">
@@ -47764,20 +47759,20 @@
       </c>
     </row>
     <row r="98" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B98" s="31" t="s">
+      <c r="B98" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C98" s="31"/>
-      <c r="D98" s="31"/>
-      <c r="E98" s="31"/>
-      <c r="F98" s="31"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
     </row>
     <row r="99" spans="2:6">
-      <c r="B99" s="31"/>
-      <c r="C99" s="31"/>
-      <c r="D99" s="31"/>
-      <c r="E99" s="31"/>
-      <c r="F99" s="31"/>
+      <c r="B99" s="32"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="32"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
     </row>
     <row r="101" spans="2:6">
       <c r="B101" s="3" t="s">
@@ -48126,27 +48121,27 @@
       </c>
     </row>
     <row r="126" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B126" s="31" t="s">
+      <c r="B126" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C126" s="31"/>
-      <c r="D126" s="31"/>
-      <c r="E126" s="31"/>
-      <c r="F126" s="31"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="32"/>
+      <c r="E126" s="32"/>
+      <c r="F126" s="32"/>
     </row>
     <row r="127" spans="2:6">
-      <c r="B127" s="31"/>
-      <c r="C127" s="31"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="31"/>
-      <c r="F127" s="31"/>
+      <c r="B127" s="32"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="32"/>
+      <c r="E127" s="32"/>
+      <c r="F127" s="32"/>
     </row>
     <row r="128" spans="2:6">
-      <c r="B128" s="31"/>
-      <c r="C128" s="31"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="31"/>
-      <c r="F128" s="31"/>
+      <c r="B128" s="32"/>
+      <c r="C128" s="32"/>
+      <c r="D128" s="32"/>
+      <c r="E128" s="32"/>
+      <c r="F128" s="32"/>
     </row>
     <row r="129" spans="2:6">
       <c r="B129" s="3" t="s">
@@ -48495,10 +48490,10 @@
       </c>
     </row>
     <row r="153" spans="2:6">
-      <c r="B153" s="27" t="s">
+      <c r="B153" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C153" s="28"/>
+      <c r="C153" s="29"/>
     </row>
     <row r="156" spans="2:6">
       <c r="B156" s="3" t="s">
@@ -48865,7 +48860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:F227"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
@@ -48889,10 +48884,10 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -49241,14 +49236,14 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="29"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -49597,20 +49592,20 @@
       </c>
     </row>
     <row r="69" spans="2:6">
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="31"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
     </row>
     <row r="70" spans="2:6">
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="3" t="s">
@@ -49959,20 +49954,20 @@
       </c>
     </row>
     <row r="96" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B96" s="32" t="s">
+      <c r="B96" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
     </row>
     <row r="97" spans="2:6">
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="33"/>
     </row>
     <row r="99" spans="2:6">
       <c r="B99" s="3" t="s">
@@ -50321,20 +50316,20 @@
       </c>
     </row>
     <row r="123" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B123" s="31" t="s">
+      <c r="B123" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C123" s="31"/>
-      <c r="D123" s="31"/>
-      <c r="E123" s="31"/>
-      <c r="F123" s="31"/>
+      <c r="C123" s="32"/>
+      <c r="D123" s="32"/>
+      <c r="E123" s="32"/>
+      <c r="F123" s="32"/>
     </row>
     <row r="124" spans="2:6">
-      <c r="B124" s="31"/>
-      <c r="C124" s="31"/>
-      <c r="D124" s="31"/>
-      <c r="E124" s="31"/>
-      <c r="F124" s="31"/>
+      <c r="B124" s="32"/>
+      <c r="C124" s="32"/>
+      <c r="D124" s="32"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
     </row>
     <row r="126" spans="2:6">
       <c r="B126" s="3" t="s">
@@ -50683,20 +50678,20 @@
       </c>
     </row>
     <row r="150" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B150" s="31" t="s">
+      <c r="B150" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C150" s="31"/>
-      <c r="D150" s="31"/>
-      <c r="E150" s="31"/>
-      <c r="F150" s="31"/>
+      <c r="C150" s="32"/>
+      <c r="D150" s="32"/>
+      <c r="E150" s="32"/>
+      <c r="F150" s="32"/>
     </row>
     <row r="151" spans="2:6">
-      <c r="B151" s="31"/>
-      <c r="C151" s="31"/>
-      <c r="D151" s="31"/>
-      <c r="E151" s="31"/>
-      <c r="F151" s="31"/>
+      <c r="B151" s="32"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="32"/>
+      <c r="E151" s="32"/>
+      <c r="F151" s="32"/>
     </row>
     <row r="153" spans="2:6">
       <c r="B153" s="3" t="s">
@@ -51045,10 +51040,10 @@
       </c>
     </row>
     <row r="176" spans="2:6">
-      <c r="B176" s="28" t="s">
+      <c r="B176" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C176" s="28"/>
+      <c r="C176" s="29"/>
     </row>
     <row r="179" spans="2:6">
       <c r="B179" s="3" t="s">
@@ -51397,14 +51392,14 @@
       </c>
     </row>
     <row r="203" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B203" s="29" t="s">
+      <c r="B203" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C203" s="29"/>
+      <c r="C203" s="30"/>
     </row>
     <row r="204" spans="2:6">
-      <c r="B204" s="30"/>
-      <c r="C204" s="30"/>
+      <c r="B204" s="31"/>
+      <c r="C204" s="31"/>
     </row>
     <row r="206" spans="2:6">
       <c r="B206" s="3" t="s">
@@ -51797,10 +51792,10 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -52149,20 +52144,20 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -52511,20 +52506,20 @@
       </c>
     </row>
     <row r="69" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
     </row>
     <row r="70" spans="2:6">
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="3" t="s">
@@ -52873,20 +52868,20 @@
       </c>
     </row>
     <row r="96" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B96" s="32" t="s">
+      <c r="B96" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="32"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
     </row>
     <row r="97" spans="2:6">
-      <c r="B97" s="32"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
+      <c r="B97" s="33"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="33"/>
     </row>
     <row r="99" spans="2:6">
       <c r="B99" s="3" t="s">
@@ -53235,20 +53230,20 @@
       </c>
     </row>
     <row r="123" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B123" s="32" t="s">
+      <c r="B123" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C123" s="32"/>
-      <c r="D123" s="32"/>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="33"/>
+      <c r="F123" s="33"/>
     </row>
     <row r="124" spans="2:6">
-      <c r="B124" s="32"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="32"/>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33"/>
     </row>
     <row r="126" spans="2:6">
       <c r="B126" s="3" t="s">
@@ -53597,20 +53592,20 @@
       </c>
     </row>
     <row r="150" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B150" s="33" t="s">
+      <c r="B150" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C150" s="33"/>
-      <c r="D150" s="33"/>
-      <c r="E150" s="33"/>
-      <c r="F150" s="33"/>
+      <c r="C150" s="34"/>
+      <c r="D150" s="34"/>
+      <c r="E150" s="34"/>
+      <c r="F150" s="34"/>
     </row>
     <row r="151" spans="2:6">
-      <c r="B151" s="33"/>
-      <c r="C151" s="33"/>
-      <c r="D151" s="33"/>
-      <c r="E151" s="33"/>
-      <c r="F151" s="33"/>
+      <c r="B151" s="34"/>
+      <c r="C151" s="34"/>
+      <c r="D151" s="34"/>
+      <c r="E151" s="34"/>
+      <c r="F151" s="34"/>
     </row>
     <row r="152" spans="2:6">
       <c r="B152" s="3" t="s">
@@ -53959,10 +53954,10 @@
       </c>
     </row>
     <row r="174" spans="2:6">
-      <c r="B174" s="28" t="s">
+      <c r="B174" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C174" s="28"/>
+      <c r="C174" s="29"/>
     </row>
     <row r="177" spans="2:6">
       <c r="B177" s="3" t="s">
@@ -54311,14 +54306,14 @@
       </c>
     </row>
     <row r="201" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B201" s="29" t="s">
+      <c r="B201" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C201" s="29"/>
+      <c r="C201" s="30"/>
     </row>
     <row r="202" spans="2:6">
-      <c r="B202" s="30"/>
-      <c r="C202" s="30"/>
+      <c r="B202" s="31"/>
+      <c r="C202" s="31"/>
     </row>
     <row r="204" spans="2:6">
       <c r="B204" s="3" t="s">
@@ -55018,10 +55013,10 @@
       </c>
     </row>
     <row r="252" spans="2:6">
-      <c r="B252" s="28" t="s">
+      <c r="B252" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C252" s="28"/>
+      <c r="C252" s="29"/>
     </row>
     <row r="255" spans="2:6">
       <c r="B255" s="3" t="s">
@@ -55370,14 +55365,14 @@
       </c>
     </row>
     <row r="279" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B279" s="29" t="s">
+      <c r="B279" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C279" s="29"/>
+      <c r="C279" s="30"/>
     </row>
     <row r="280" spans="2:6">
-      <c r="B280" s="30"/>
-      <c r="C280" s="30"/>
+      <c r="B280" s="31"/>
+      <c r="C280" s="31"/>
     </row>
     <row r="282" spans="2:6">
       <c r="B282" s="3" t="s">
@@ -56078,16 +56073,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B42:F43"/>
+    <mergeCell ref="B69:F70"/>
+    <mergeCell ref="B96:F97"/>
+    <mergeCell ref="B123:F124"/>
     <mergeCell ref="B252:C252"/>
     <mergeCell ref="B279:C280"/>
     <mergeCell ref="B174:C174"/>
     <mergeCell ref="B201:C202"/>
     <mergeCell ref="B150:F151"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B42:F43"/>
-    <mergeCell ref="B69:F70"/>
-    <mergeCell ref="B96:F97"/>
-    <mergeCell ref="B123:F124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -56099,7 +56094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A15:F390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A360" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView topLeftCell="A275" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="H382" sqref="H382"/>
     </sheetView>
   </sheetViews>
@@ -56113,20 +56108,20 @@
   </cols>
   <sheetData>
     <row r="15" spans="2:6">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="3" t="s">
@@ -56475,20 +56470,20 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3" t="s">
@@ -56837,20 +56832,20 @@
       </c>
     </row>
     <row r="69" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
     </row>
     <row r="70" spans="2:6">
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="3" t="s">
@@ -57199,20 +57194,20 @@
       </c>
     </row>
     <row r="95" spans="2:6" ht="42.75" customHeight="1">
-      <c r="B95" s="31" t="s">
+      <c r="B95" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C95" s="31"/>
-      <c r="D95" s="31"/>
-      <c r="E95" s="31"/>
-      <c r="F95" s="31"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
     </row>
     <row r="96" spans="2:6">
-      <c r="B96" s="31"/>
-      <c r="C96" s="31"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="31"/>
-      <c r="F96" s="31"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
     </row>
     <row r="98" spans="2:6">
       <c r="B98" s="3" t="s">
@@ -57561,14 +57556,14 @@
       </c>
     </row>
     <row r="122" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B122" s="29" t="s">
+      <c r="B122" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C122" s="29"/>
+      <c r="C122" s="30"/>
     </row>
     <row r="123" spans="2:6">
-      <c r="B123" s="30"/>
-      <c r="C123" s="30"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="31"/>
     </row>
     <row r="125" spans="2:6">
       <c r="B125" s="3" t="s">
@@ -58268,10 +58263,10 @@
       </c>
     </row>
     <row r="174" spans="2:6">
-      <c r="B174" s="27" t="s">
+      <c r="B174" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C174" s="28"/>
+      <c r="C174" s="29"/>
     </row>
     <row r="177" spans="2:6">
       <c r="B177" s="3" t="s">
@@ -58620,14 +58615,14 @@
       </c>
     </row>
     <row r="201" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B201" s="29" t="s">
+      <c r="B201" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C201" s="29"/>
+      <c r="C201" s="30"/>
     </row>
     <row r="202" spans="2:6">
-      <c r="B202" s="30"/>
-      <c r="C202" s="30"/>
+      <c r="B202" s="31"/>
+      <c r="C202" s="31"/>
     </row>
     <row r="204" spans="2:6">
       <c r="B204" s="3" t="s">
@@ -59326,14 +59321,14 @@
       </c>
     </row>
     <row r="256" spans="2:6" ht="14.25" customHeight="1">
-      <c r="B256" s="29" t="s">
+      <c r="B256" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C256" s="29"/>
+      <c r="C256" s="30"/>
     </row>
     <row r="257" spans="2:6">
-      <c r="B257" s="30"/>
-      <c r="C257" s="30"/>
+      <c r="B257" s="31"/>
+      <c r="C257" s="31"/>
     </row>
     <row r="259" spans="2:6">
       <c r="B259" s="3" t="s">
@@ -59683,10 +59678,10 @@
     </row>
     <row r="283" spans="1:6">
       <c r="A283" s="20"/>
-      <c r="B283" s="27" t="s">
+      <c r="B283" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C283" s="28"/>
+      <c r="C283" s="29"/>
       <c r="D283" s="20"/>
       <c r="E283" s="21"/>
       <c r="F283" s="20"/>
@@ -60077,18 +60072,18 @@
     </row>
     <row r="310" spans="1:6">
       <c r="A310" s="20"/>
-      <c r="B310" s="29" t="s">
+      <c r="B310" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C310" s="29"/>
+      <c r="C310" s="30"/>
       <c r="D310" s="22"/>
       <c r="E310" s="22"/>
       <c r="F310" s="22"/>
     </row>
     <row r="311" spans="1:6">
       <c r="A311" s="20"/>
-      <c r="B311" s="30"/>
-      <c r="C311" s="30"/>
+      <c r="B311" s="31"/>
+      <c r="C311" s="31"/>
       <c r="D311" s="22"/>
       <c r="E311" s="22"/>
       <c r="F311" s="22"/>
@@ -60873,18 +60868,18 @@
     </row>
     <row r="365" spans="1:6">
       <c r="A365" s="20"/>
-      <c r="B365" s="29" t="s">
+      <c r="B365" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C365" s="29"/>
+      <c r="C365" s="30"/>
       <c r="D365" s="22"/>
       <c r="E365" s="22"/>
       <c r="F365" s="22"/>
     </row>
     <row r="366" spans="1:6">
       <c r="A366" s="20"/>
-      <c r="B366" s="30"/>
-      <c r="C366" s="30"/>
+      <c r="B366" s="31"/>
+      <c r="C366" s="31"/>
       <c r="D366" s="22"/>
       <c r="E366" s="22"/>
       <c r="F366" s="22"/>
@@ -60915,10 +60910,10 @@
     </row>
     <row r="369" spans="1:6">
       <c r="A369" s="20"/>
-      <c r="B369" s="34">
+      <c r="B369" s="27">
         <v>4.8872947692870997E-2</v>
       </c>
-      <c r="C369" s="34">
+      <c r="C369" s="27">
         <v>1</v>
       </c>
       <c r="D369" s="22"/>
@@ -61259,17 +61254,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B15:F16"/>
-    <mergeCell ref="B42:F43"/>
-    <mergeCell ref="B69:F70"/>
-    <mergeCell ref="B95:F96"/>
-    <mergeCell ref="B122:C123"/>
     <mergeCell ref="B365:C366"/>
     <mergeCell ref="B283:C283"/>
     <mergeCell ref="B310:C311"/>
     <mergeCell ref="B174:C174"/>
     <mergeCell ref="B201:C202"/>
     <mergeCell ref="B256:C257"/>
+    <mergeCell ref="B15:F16"/>
+    <mergeCell ref="B42:F43"/>
+    <mergeCell ref="B69:F70"/>
+    <mergeCell ref="B95:F96"/>
+    <mergeCell ref="B122:C123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>